<commit_message>
excel: sorting & filtering
</commit_message>
<xml_diff>
--- a/02_preparing_data_with_excel/Sample.xlsx
+++ b/02_preparing_data_with_excel/Sample.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EBBDEC-E88C-4AC0-8810-29119589F148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD4468D-C112-460E-B8C8-987B582814A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0810452C-9FFD-4B22-AA5E-32A4DA9D959D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0810452C-9FFD-4B22-AA5E-32A4DA9D959D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Figures" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
   <si>
     <t>City</t>
   </si>
@@ -197,9 +197,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -259,9 +259,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B113F36-E1CD-49EA-93F9-DD60CDD9FDB1}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,7 +1116,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1197,7 +1200,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1286,10 +1291,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D018C0-3468-48E5-ADA7-F7B9F33F18F5}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,6 +1344,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FC33AF-F89E-4C17-8BA2-B6D77F587361}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1486,26 +1493,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EAC3B332A2FD04E918F9FD72E2B30AC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5791f7a1e5ce60c682c7fd472657cfed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aed4346-8012-4133-9837-e496d0f5c99a" xmlns:ns3="15179a99-4cef-4bac-ab20-a4c03d7ec5db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4db72e02b896ab7bb9242ff846c9720" ns2:_="" ns3:_="">
     <xsd:import namespace="2aed4346-8012-4133-9837-e496d0f5c99a"/>
@@ -1722,32 +1709,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC6A9E-AFDB-4CBD-9896-E5C36F677490}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACFCDE67-DA47-4FB4-981D-4C7D3281006C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFCCA327-4613-4AB7-899B-CACED6736245}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1764,4 +1746,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACFCDE67-DA47-4FB4-981D-4C7D3281006C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC6A9E-AFDB-4CBD-9896-E5C36F677490}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>